<commit_message>
Intégration article 6 (mais retouches à faire)
La plupart des augmentations ont été placées, mais il faudra les revoir
</commit_message>
<xml_diff>
--- a/content/06/augmentations/ART06-augm.xlsx
+++ b/content/06/augmentations/ART06-augm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -62,7 +62,7 @@
     <t xml:space="preserve">year</t>
   </si>
   <si>
-    <t xml:space="preserve">Fichier média + emplacement</t>
+    <t xml:space="preserve">src</t>
   </si>
   <si>
     <t xml:space="preserve">medium</t>
@@ -2118,8 +2118,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3082,7 +3082,7 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>